<commit_message>
add test skip lines
</commit_message>
<xml_diff>
--- a/src/main/resources/excel-all-formats-test.xlsx
+++ b/src/main/resources/excel-all-formats-test.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Plan1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Plan1!$A$1:$BJ$206</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Plan1!$A$1:$BJ$207</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -365,10 +365,10 @@
   </sheetPr>
   <dimension ref="A1:I65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -539,87 +539,97 @@
       <c r="I5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>42498</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>100000</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F6" s="8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="10" t="n">
-        <v>42498.5932175926</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
       <c r="I6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>42499</v>
+        <v>42498</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" s="7" t="n">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="F7" s="8" t="n">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H7" s="10" t="n">
-        <v>42499.6355902778</v>
+        <v>42498.5932175926</v>
       </c>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="n">
-        <v>42500</v>
+        <v>42499</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" s="7" t="n">
-        <v>100000000</v>
+        <v>1000000</v>
       </c>
       <c r="F8" s="8" t="n">
-        <v>100000</v>
+        <v>10000</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H8" s="10" t="n">
-        <v>42500.677962963</v>
+        <v>42499.6355902778</v>
       </c>
       <c r="I8" s="11"/>
     </row>
-    <row r="1048364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>42500</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>100000000</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>100000</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="10" t="n">
+        <v>42500.677962963</v>
+      </c>
+      <c r="I9" s="11"/>
+    </row>
     <row r="1048365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>